<commit_message>
Add watermark on image.
</commit_message>
<xml_diff>
--- a/Content/Tractors/Tractor_Image_Infos.xlsx
+++ b/Content/Tractors/Tractor_Image_Infos.xlsx
@@ -14,48 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mahindra Tractors</t>
   </si>
   <si>
-    <t>Farmtrac Tractors</t>
-  </si>
-  <si>
-    <t>Kubota Tractors</t>
-  </si>
-  <si>
-    <t>Powertrac Tractors</t>
-  </si>
-  <si>
     <t>ARJUN NOVO 605 DI–i-4WD</t>
   </si>
   <si>
-    <t>60 PowerMaxx</t>
-  </si>
-  <si>
-    <t>MU4501 2WD</t>
-  </si>
-  <si>
-    <t>265 DI</t>
-  </si>
-  <si>
-    <t>Euro 50</t>
-  </si>
-  <si>
     <t>['img0-mahindra-arjun-novo-605-dii-4wd-1698917936.png', 'img1-mahindra-arjun-novo-605-dii-4wd-16989179360.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-farmtrac-60-powermaxx-1690541201.png', 'img1-farmtrac-60-powermaxx-16905412010.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-kubota-mu4501-2wd.png', 'img1-upload-1632223345-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-265-di-1632210883.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-265-di-1632210883.png']</t>
-  </si>
-  <si>
-    <t>['img0-euro-50-1632287717.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -420,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,13 +395,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -442,54 +409,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created logic for add watermark and harvester.
</commit_message>
<xml_diff>
--- a/Content/Tractors/Tractor_Image_Infos.xlsx
+++ b/Content/Tractors/Tractor_Image_Infos.xlsx
@@ -14,15 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Mahindra Tractors</t>
   </si>
   <si>
+    <t>Swaraj Tractors</t>
+  </si>
+  <si>
+    <t>John Deere Tractors</t>
+  </si>
+  <si>
     <t>ARJUN NOVO 605 DI–i-4WD</t>
   </si>
   <si>
+    <t>855 FE</t>
+  </si>
+  <si>
+    <t>265 DI</t>
+  </si>
+  <si>
+    <t>5050 D</t>
+  </si>
+  <si>
+    <t>Yuvraj 215 NXT</t>
+  </si>
+  <si>
     <t>['img0-mahindra-arjun-novo-605-dii-4wd-1698917936.png', 'img1-mahindra-arjun-novo-605-dii-4wd-16989179360.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-swaraj-855-fe-1694259363.png', 'img1-855-fe-1631015724.png', 'img2-upload-1631015724-0.png', 'img3-swaraj-855-fe-16942593630.png']</t>
+  </si>
+  <si>
+    <t>['img0-265-di-1632210883.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-265-di-1632210883.png']</t>
+  </si>
+  <si>
+    <t>['img0-5050-d-1632220934.png', 'img1-upload-1632220934-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['img0-yuvraj-215-nxt-1632209478.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -387,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,13 +425,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -409,10 +439,54 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scraped the tyre data.
</commit_message>
<xml_diff>
--- a/Content/Tractors/Tractor_Image_Infos.xlsx
+++ b/Content/Tractors/Tractor_Image_Infos.xlsx
@@ -14,45 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Mahindra Tractors</t>
   </si>
   <si>
-    <t>Swaraj Tractors</t>
-  </si>
-  <si>
-    <t>John Deere Tractors</t>
-  </si>
-  <si>
-    <t>ARJUN NOVO 605 DI–i-4WD</t>
-  </si>
-  <si>
-    <t>855 FE</t>
-  </si>
-  <si>
-    <t>265 DI</t>
-  </si>
-  <si>
-    <t>5050 D</t>
-  </si>
-  <si>
-    <t>Yuvraj 215 NXT</t>
-  </si>
-  <si>
-    <t>['img0-mahindra-arjun-novo-605-dii-4wd-1698917936.png', 'img1-mahindra-arjun-novo-605-dii-4wd-16989179360.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-swaraj-855-fe-1694259363.png', 'img1-855-fe-1631015724.png', 'img2-upload-1631015724-0.png', 'img3-swaraj-855-fe-16942593630.png']</t>
-  </si>
-  <si>
-    <t>['img0-265-di-1632210883.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-265-di-1632210883.png']</t>
-  </si>
-  <si>
-    <t>['img0-5050-d-1632220934.png', 'img1-upload-1632220934-0.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
-  </si>
-  <si>
-    <t>['img0-yuvraj-215-nxt-1632209478.png', 'img1-mqdefault.png', 'img2-mqdefault.png', 'img3-mqdefault.png']</t>
+    <t>275 DI TU XP Plus</t>
+  </si>
+  <si>
+    <t>Arjun 555 DI</t>
+  </si>
+  <si>
+    <t>['275 DI TU XP Plusimg0-275-di-tu-xp-plus-1632304804.png', '275 DI TU XP Plusimg1-275-di-tu-xp-plus-1632304804.png', '275 DI TU XP Plusimg2-mqdefault.png']</t>
+  </si>
+  <si>
+    <t>['Arjun 555 DIimg0-arjun-555-di-1632207634.png', 'Arjun 555 DIimg1-mqdefault.png', 'Arjun 555 DIimg2-mqdefault.png', 'Arjun 555 DIimg3-arjun-555-di-1632207634.png']</t>
   </si>
   <si>
     <t>Brand</t>
@@ -417,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,13 +401,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -439,54 +415,21 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>